<commit_message>
add teh umovy elektrika
add teh umovy elektrika
</commit_message>
<xml_diff>
--- a/муровка/вартість_квадрату_добудови.xlsx
+++ b/муровка/вартість_квадрату_добудови.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20730" windowHeight="10050" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="20730" windowHeight="10050" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="підїзд1" sheetId="1" r:id="rId1"/>
@@ -1892,8 +1892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O76"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView topLeftCell="C34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3585,8 +3585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4915,8 +4915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:N62"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6741,7 +6741,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26:C27"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7767,8 +7767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:I7"/>
+    <sheetView topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>